<commit_message>
CCDB-274: Using the new template.
</commit_message>
<xml_diff>
--- a/conf-core/src/main/webapp/resources/import-templates/ccdb_properties.xlsx
+++ b/conf-core/src/main/webapp/resources/import-templates/ccdb_properties.xlsx
@@ -9,17 +9,56 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="135" windowWidth="37395" windowHeight="17940"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995"/>
   </bookViews>
   <sheets>
-    <sheet name="Units" sheetId="1" r:id="rId1"/>
+    <sheet name="Properties" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Version</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Copyright</t>
+  </si>
+  <si>
+    <t>License</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>OPERATION</t>
+  </si>
+  <si>
+    <t>LGPL3</t>
+  </si>
+  <si>
+    <t>Create</t>
+  </si>
+  <si>
+    <t>Update</t>
+  </si>
+  <si>
+    <t>Delete</t>
+  </si>
+  <si>
+    <t>European Spallation Source (ESS)</t>
+  </si>
+  <si>
+    <t>2015/MAY/06</t>
+  </si>
   <si>
     <t>NAME</t>
   </si>
@@ -27,28 +66,22 @@
     <t>DESCRIPTION</t>
   </si>
   <si>
-    <t>OPERATION</t>
-  </si>
-  <si>
-    <t>Version</t>
-  </si>
-  <si>
-    <t>Date</t>
-  </si>
-  <si>
-    <t>Description</t>
+    <t>Total names</t>
   </si>
   <si>
     <t>1.0</t>
   </si>
   <si>
-    <t>Import properties file</t>
+    <t>Production</t>
+  </si>
+  <si>
+    <t>Template file to import properties in the CCDB</t>
+  </si>
+  <si>
+    <t>DATA TYPE</t>
   </si>
   <si>
     <t>UNIT</t>
-  </si>
-  <si>
-    <t>DATA TYPE</t>
   </si>
   <si>
     <t>UNIQUENESS</t>
@@ -58,12 +91,20 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -84,7 +125,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="3" tint="0.79998168889431442"/>
+        <fgColor theme="3" tint="0.59996337778862885"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -116,28 +157,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1"/>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -442,122 +471,141 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F6" sqref="F6"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="30.7109375" defaultRowHeight="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.7109375" style="9"/>
-    <col min="2" max="5" width="20.7109375" style="8"/>
-    <col min="6" max="16384" width="20.7109375" style="1"/>
+    <col min="1" max="1" width="30.7109375" style="3"/>
+    <col min="4" max="4" width="30.7109375" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="2" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:6" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1">
+        <f xml:space="preserve"> SUMPRODUCT((B9:B65536 &lt;&gt; "") / COUNTIF(B9:B65536, B9:B65536 &amp; ""))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2">
+        <f xml:space="preserve"> COUNTIF(A8:A65536, "CREATE")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3">
+        <f xml:space="preserve"> COUNTIF(A8:A65536, "UPDATE")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4">
+        <f xml:space="preserve"> COUNTIF(A8:A65536, "DELETE")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="10">
-        <v>42116</v>
-      </c>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-    </row>
-    <row r="2" spans="1:6" s="2" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="4" t="s">
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="21.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="8" spans="1:6" ht="21.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-    </row>
-    <row r="3" spans="1:6" s="2" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-    </row>
-    <row r="4" spans="1:6" s="2" customFormat="1" ht="21.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="5"/>
-      <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-    </row>
-    <row r="5" spans="1:6" s="2" customFormat="1" ht="21.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="F5" s="6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="7"/>
-    </row>
-    <row r="7" spans="1:6" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="7"/>
+      <c r="B8" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="6"/>
+      <c r="D9" s="4"/>
+    </row>
+    <row r="10" spans="1:6" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="4"/>
+      <c r="D10" s="4"/>
+    </row>
+    <row r="11" spans="1:6" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="4"/>
+      <c r="E11" s="3"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="ilc2eqh5wj/Ej0DJj/iS1DFN7x9ZSaYQLTmwSaulkBkcshDEsJmBz7FO0b1vUtCJuzLIFeu6B6+5lww8lJMveQ==" saltValue="Ntwrr/px6+EEweVT4ijVKA==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
-  <protectedRanges>
-    <protectedRange algorithmName="SHA-512" hashValue="EeGo8NBC4pNhZULZNaKuYvDytr72sNAZGKPQclUfebB9p1K/COIIzmq7ypdmWUrLgKG8YSgznzmYVgZcEd9pmw==" saltValue="ZUQ9+Q/Q4L3Ixt2ynw4A8w==" spinCount="100000" sqref="A1:XFD5" name="Locked header cells"/>
-  </protectedRanges>
-  <dataValidations count="12">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A6:A1048576">
-      <formula1>"CREATE,UPDATE,DELETE,END"</formula1>
+  <dataValidations count="5">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Lorem Ipsum" sqref="B8:C8 F8"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Lorem Ipsum" sqref="D8:E8"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A9:A1048576">
+      <formula1>"CREATE,UPDATE,DELETE"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Select one of the possible import operations. If left blank, this line will not be imported. _x000a_This column is not imported into the database; it controls the import process." sqref="A5"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Property name (REQUIRED)" prompt="The unique name of the property" sqref="B5"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Uniqueness (REQUIRED)" prompt="Defines whether the value of the property is _x000a_- unique accross all values for the same property in the database, _x000a_- only for values of the same property for the entities of the same device type, or _x000a_- the values are not checked for uniqueness." sqref="F5"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Data type (REQUIRED)" prompt="The name of the data type._x000a_Must equal to the name of the user defined or built-in data type._x000a_Built-in data types are:_x000a_  Integer_x000a_  Double_x000a_  String_x000a_  Timestamp_x000a_  Integers Vector_x000a_  Doubles Vector_x000a_  Strings List_x000a_  Doubles Table" sqref="E5"/>
-    <dataValidation type="textLength" allowBlank="1" showErrorMessage="1" errorTitle="Invalid length" error="The property name must be between 1 and 64 characters long." sqref="B6:B1048576">
-      <formula1>1</formula1>
-      <formula2>64</formula2>
-    </dataValidation>
-    <dataValidation type="textLength" allowBlank="1" showErrorMessage="1" errorTitle="Invalid length" error="The property description must be between 1 and 64 characters long." sqref="C6:C1048576">
-      <formula1>1</formula1>
-      <formula2>255</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Property description (REQUIRED)" prompt="The description of the property for the user." sqref="C5"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Unit name" prompt="The optional unit for this property._x000a_The name of the unit MUST equal to one of the defined units." sqref="D5"/>
-    <dataValidation type="textLength" allowBlank="1" showErrorMessage="1" errorTitle="Invalid length" error="The data type name must be between 1 and 64 characters long." sqref="E6:E1048576">
-      <formula1>1</formula1>
-      <formula2>64</formula2>
-    </dataValidation>
-    <dataValidation type="textLength" allowBlank="1" showErrorMessage="1" errorTitle="Invalid length" error="The unit name must be between 1 and 32 characters long." sqref="D6:D1048576">
-      <formula1>1</formula1>
-      <formula2>32</formula2>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F6:F1048576">
-      <formula1>"UNIVERSAL,TYPE,NONE"</formula1>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Lorem Ipsum" sqref="A8"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F9:F1048576">
+      <formula1>"NONE,TYPE,UNIVERSAL"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="B2" numberStoredAsText="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>